<commit_message>
Update enumerator names post training
</commit_message>
<xml_diff>
--- a/ILRG_Hluvukani_A_encontros/ILRG_Hluvukani_A_encontros-media/ILRG_Hluvukani_A_encontros.xlsx
+++ b/ILRG_Hluvukani_A_encontros/ILRG_Hluvukani_A_encontros-media/ILRG_Hluvukani_A_encontros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\Grants\Hluvukani\ODK Forms\ILRG_hluvukani_odk_forms\ILRG_Hluvukani_A_encontros\ILRG_Hluvukani_A_encontros-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD804ECA-354F-44C6-9D0B-2D6125617DD9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A267EA18-D249-43C6-861C-D6ADF17542B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">choices!$A$1:$C$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">choices!$A$1:$C$16</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="231">
   <si>
     <t>type</t>
   </si>
@@ -355,15 +355,6 @@
   </si>
   <si>
     <t>Taninga South</t>
-  </si>
-  <si>
-    <t>Palmeira 1</t>
-  </si>
-  <si>
-    <t>Palmeira 2</t>
-  </si>
-  <si>
-    <t>Palmeira 3</t>
   </si>
   <si>
     <t>Manhiça Municipality</t>
@@ -720,109 +711,89 @@
     <t>Boaventura Jovo</t>
   </si>
   <si>
-    <t>Carlos Munjovo</t>
-  </si>
-  <si>
-    <t>Edmilson Momade</t>
-  </si>
-  <si>
-    <t>Edson Adozinda</t>
-  </si>
-  <si>
-    <t>Efigencia Alberto</t>
-  </si>
-  <si>
-    <t>Ester Matlombe</t>
-  </si>
-  <si>
-    <t>Herondina Timane</t>
-  </si>
-  <si>
-    <t>Irene Timane</t>
-  </si>
-  <si>
     <t>Julio Manheia</t>
   </si>
   <si>
-    <t>Ossifo Pinto</t>
-  </si>
-  <si>
     <t>Raquel Ambasse</t>
   </si>
   <si>
-    <t>Sandra Dimande</t>
-  </si>
-  <si>
     <t>Boaventura_Jovo</t>
   </si>
   <si>
-    <t>Carlos_Munjovo</t>
-  </si>
-  <si>
-    <t>Edmilson_Momade</t>
-  </si>
-  <si>
-    <t>Edson_Adozinda</t>
-  </si>
-  <si>
-    <t>Efigencia_Alberto</t>
-  </si>
-  <si>
-    <t>Ester_Matlombe</t>
-  </si>
-  <si>
-    <t>Herondina_Timane</t>
-  </si>
-  <si>
-    <t>Irene_Timane</t>
-  </si>
-  <si>
     <t>Julio_Manheia</t>
   </si>
   <si>
-    <t>Ossifo_Pinto</t>
-  </si>
-  <si>
     <t>Raquel_Ambasse</t>
   </si>
   <si>
-    <t>Sandra_Dimande</t>
-  </si>
-  <si>
     <t>Helena_Bila</t>
   </si>
   <si>
     <t>Armando_Zuana</t>
   </si>
   <si>
-    <t>Gercia_A.Mabunda</t>
-  </si>
-  <si>
-    <t>Guilherme_Nhacundela</t>
-  </si>
-  <si>
     <t>Armando Zuana</t>
   </si>
   <si>
-    <t>Gercia A.Mabunda</t>
-  </si>
-  <si>
-    <t>Guilherme Nhacundela</t>
-  </si>
-  <si>
     <t>Helena Bila</t>
   </si>
   <si>
     <t>meet_municipality</t>
+  </si>
+  <si>
+    <t>Carlos_Mujovo</t>
+  </si>
+  <si>
+    <t>Carlos Mujovo</t>
+  </si>
+  <si>
+    <t>Edson Ernesto</t>
+  </si>
+  <si>
+    <t>Edson_Ernesto</t>
+  </si>
+  <si>
+    <t>Efigencia Mavondza</t>
+  </si>
+  <si>
+    <t>Efigencia_Mavondza</t>
+  </si>
+  <si>
+    <t>Gercia_Mabunda</t>
+  </si>
+  <si>
+    <t>Gercia Mabunda</t>
+  </si>
+  <si>
+    <t>Irene Timana</t>
+  </si>
+  <si>
+    <t>Irene_Timana</t>
+  </si>
+  <si>
+    <t>Palmeira Norte</t>
+  </si>
+  <si>
+    <t>Palmeira Centro</t>
+  </si>
+  <si>
+    <t>Palmeira Sul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1060,354 +1031,362 @@
   </borders>
   <cellStyleXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="234" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="234" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="236">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1984,7 +1963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2068,13 +2047,13 @@
     </row>
     <row r="4" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2085,7 +2064,7 @@
         <v>83</v>
       </c>
       <c r="M5" s="51" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2093,7 +2072,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C6" s="2"/>
       <c r="L6" s="43" t="s">
@@ -2105,10 +2084,10 @@
         <v>45</v>
       </c>
       <c r="B7" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="N7" s="43" t="s">
         <v>140</v>
-      </c>
-      <c r="N7" s="43" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2116,10 +2095,10 @@
         <v>45</v>
       </c>
       <c r="B8" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>141</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2136,7 +2115,7 @@
         <v>46</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2144,7 +2123,7 @@
         <v>64</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>44</v>
@@ -2161,13 +2140,13 @@
         <v>25</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L12" s="43" t="s">
         <v>35</v>
@@ -2178,13 +2157,13 @@
         <v>32</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H13" s="43" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J13" s="43" t="s">
         <v>23</v>
@@ -2195,13 +2174,13 @@
         <v>32</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H14" s="43" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J14" s="43" t="s">
         <v>23</v>
@@ -2249,16 +2228,16 @@
     </row>
     <row r="18" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C18" s="31" t="s">
         <v>94</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>23</v>
@@ -2272,10 +2251,10 @@
         <v>25</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2288,7 +2267,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>39</v>
@@ -2302,7 +2281,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="44" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>40</v>
@@ -2322,7 +2301,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="44" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C23" s="31" t="s">
         <v>38</v>
@@ -2336,16 +2315,16 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B24" s="44" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C24" s="31" t="s">
         <v>41</v>
       </c>
       <c r="G24" s="43" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
@@ -2365,19 +2344,19 @@
         <v>32</v>
       </c>
       <c r="B25" s="44" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G25" s="43" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H25" s="25" t="s">
         <v>74</v>
       </c>
       <c r="I25" s="31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>23</v>
@@ -2391,7 +2370,7 @@
         <v>72</v>
       </c>
       <c r="B26" s="44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C26" s="31" t="s">
         <v>58</v>
@@ -2405,19 +2384,19 @@
         <v>32</v>
       </c>
       <c r="B27" s="44" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G27" s="43" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H27" s="25" t="s">
         <v>74</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>23</v>
@@ -2428,7 +2407,7 @@
         <v>43</v>
       </c>
       <c r="B28" s="44" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>61</v>
@@ -2445,19 +2424,19 @@
         <v>32</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>62</v>
       </c>
       <c r="G29" s="43" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H29" s="25" t="s">
         <v>74</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J29" s="20" t="s">
         <v>23</v>
@@ -2468,7 +2447,7 @@
         <v>25</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>81</v>
@@ -2483,7 +2462,7 @@
         <v>66</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>77</v>
@@ -2500,7 +2479,7 @@
         <v>66</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>78</v>
@@ -2517,7 +2496,7 @@
         <v>66</v>
       </c>
       <c r="B33" s="44" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C33" s="31" t="s">
         <v>79</v>
@@ -2542,10 +2521,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="44" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J35" s="25" t="s">
         <v>23</v>
@@ -2556,10 +2535,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>36</v>
@@ -2576,13 +2555,13 @@
         <v>60</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H37" s="25" t="s">
         <v>74</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J37" s="31" t="s">
         <v>23</v>
@@ -2608,13 +2587,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:C19"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,10 +2630,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2662,10 +2641,10 @@
         <v>18</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J4" s="31"/>
     </row>
@@ -2673,44 +2652,45 @@
       <c r="A5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="52" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" s="56" t="s">
-        <v>211</v>
+      <c r="B5" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>224</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="52" t="s">
-        <v>225</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>213</v>
-      </c>
+      <c r="B7" s="60" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>214</v>
+      <c r="B8" s="60" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>225</v>
       </c>
       <c r="J8" s="3"/>
     </row>
@@ -2718,11 +2698,11 @@
       <c r="A9" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>227</v>
+      <c r="B9" s="54" t="s">
+        <v>213</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J9" s="3"/>
     </row>
@@ -2730,11 +2710,11 @@
       <c r="A10" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="54" t="s">
-        <v>236</v>
-      </c>
-      <c r="C10" s="53" t="s">
-        <v>239</v>
+      <c r="B10" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>226</v>
       </c>
       <c r="J10" s="3"/>
     </row>
@@ -2742,357 +2722,359 @@
       <c r="A11" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="54" t="s">
-        <v>237</v>
+      <c r="B11" s="47" t="s">
+        <v>211</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>240</v>
-      </c>
-      <c r="J11" s="3"/>
+        <v>208</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="54" t="s">
-        <v>234</v>
+      <c r="B12" s="33" t="s">
+        <v>212</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>241</v>
-      </c>
-      <c r="J12" s="3"/>
+        <v>209</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="54" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="30"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="C13" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="32" t="s">
+      <c r="D24" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="C14" s="53" t="s">
-        <v>217</v>
-      </c>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="47" t="s">
+      <c r="D25" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="C15" s="53" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="C16" s="53" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>232</v>
-      </c>
-      <c r="C17" s="53" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="C18" s="53" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="54" t="s">
-        <v>184</v>
-      </c>
-      <c r="C19" s="53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="30"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="47" t="s">
+      <c r="D26" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="32" t="s">
+      <c r="B27" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="32" t="s">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" s="48"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C31" s="34" t="s">
         <v>111</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="F31" s="48"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B32" s="37" t="s">
-        <v>99</v>
+        <v>147</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>107</v>
       </c>
       <c r="C32" s="34" t="s">
         <v>112</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>86</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F32" s="48"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="F33" s="48"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="A34" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="48"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="A35" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="47"/>
+      <c r="F35" s="48"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="48" t="s">
-        <v>148</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="A36" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="47"/>
       <c r="F36" s="48"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F37" s="48"/>
+      <c r="A37" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F38" s="48"/>
+      <c r="A38" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="48"/>
+      <c r="A39" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="47" t="s">
-        <v>180</v>
+      <c r="B40" s="54" t="s">
+        <v>217</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="F40" s="48"/>
+        <v>122</v>
+      </c>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B41" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="E41" s="47"/>
-      <c r="F41" s="48"/>
+        <v>123</v>
+      </c>
+      <c r="E41" s="49"/>
+      <c r="F41" s="50"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
@@ -3102,340 +3084,298 @@
         <v>181</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="E42" s="47"/>
-      <c r="F42" s="48"/>
+        <v>55</v>
+      </c>
+      <c r="E42" s="49"/>
+      <c r="F42" s="50"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="47" t="s">
-        <v>182</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>80</v>
-      </c>
+      <c r="A43" s="12"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="50"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>57</v>
+      <c r="A44" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="B44" s="47" t="s">
-        <v>183</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>123</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" s="49"/>
+      <c r="F44" s="50"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
-        <v>57</v>
+      <c r="A45" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="B45" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="C45" s="35" t="s">
-        <v>124</v>
-      </c>
+      <c r="C45" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="49"/>
+      <c r="F45" s="50"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B46" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="C46" s="35" t="s">
-        <v>125</v>
+      <c r="A46" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>76</v>
       </c>
       <c r="E46" s="49"/>
       <c r="F46" s="50"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="C47" s="35" t="s">
+      <c r="A47" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="49" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" s="34" t="s">
         <v>126</v>
       </c>
       <c r="E47" s="49"/>
       <c r="F47" s="50"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="C48" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="49"/>
-      <c r="F48" s="50"/>
+      <c r="A48" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="F48" s="48"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="50"/>
+      <c r="A49" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="F49" s="48"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="47" t="s">
-        <v>188</v>
+      <c r="B50" s="49" t="s">
+        <v>181</v>
       </c>
       <c r="C50" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="E50" s="49"/>
-      <c r="F50" s="50"/>
+        <v>55</v>
+      </c>
+      <c r="F50" s="48"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="C51" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="E51" s="49"/>
-      <c r="F51" s="50"/>
+      <c r="B51" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="48"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="49" t="s">
-        <v>190</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="E52" s="49"/>
-      <c r="F52" s="50"/>
+      <c r="A52" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="48"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B53" s="49" t="s">
-        <v>191</v>
-      </c>
-      <c r="C53" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="E53" s="49"/>
-      <c r="F53" s="50"/>
+      <c r="A53" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B53" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F53" s="48"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B54" s="49" t="s">
+      <c r="A54" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="C54" s="34" t="s">
-        <v>130</v>
+      <c r="C54" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="F54" s="48"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="49" t="s">
-        <v>192</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>131</v>
+      <c r="A55" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="F55" s="48"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="49" t="s">
-        <v>184</v>
-      </c>
-      <c r="C56" s="34" t="s">
-        <v>55</v>
+      <c r="A56" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>48</v>
       </c>
       <c r="F56" s="48"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="F57" s="48"/>
+      <c r="A57" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B58" s="47" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C58" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F58" s="48"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B59" s="47" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="F59" s="48"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B60" s="47" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="F60" s="48"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="C61" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F61" s="48"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="34" t="s">
-        <v>117</v>
+      <c r="A62" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B62" s="47" t="s">
-        <v>198</v>
-      </c>
-      <c r="C62" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F62" s="48"/>
+        <v>199</v>
+      </c>
+      <c r="C62" s="23" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="34" t="s">
-        <v>117</v>
+      <c r="A63" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B63" s="47" t="s">
-        <v>199</v>
-      </c>
-      <c r="C63" s="35" t="s">
-        <v>49</v>
+        <v>200</v>
+      </c>
+      <c r="C63" s="23" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
-        <v>117</v>
+      <c r="A64" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B64" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="C64" s="35" t="s">
-        <v>52</v>
+        <v>201</v>
+      </c>
+      <c r="C64" s="23" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
-        <v>117</v>
+      <c r="A65" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B65" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="C65" s="35" t="s">
-        <v>47</v>
+        <v>202</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
-        <v>117</v>
+      <c r="A66" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B66" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="C66" s="35" t="s">
-        <v>56</v>
+        <v>203</v>
+      </c>
+      <c r="C66" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="C68" s="23" t="s">
-        <v>67</v>
-      </c>
+      <c r="A68" s="26"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="27"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="C69" s="23" t="s">
-        <v>68</v>
-      </c>
+      <c r="A69" s="26"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="27"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" s="47" t="s">
-        <v>204</v>
-      </c>
-      <c r="C70" s="23" t="s">
-        <v>69</v>
-      </c>
+      <c r="A70" s="26"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="27"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B71" s="47" t="s">
-        <v>205</v>
-      </c>
-      <c r="C71" s="23" t="s">
-        <v>71</v>
-      </c>
+      <c r="A71" s="26"/>
+      <c r="B71" s="38"/>
+      <c r="C71" s="27"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B72" s="47" t="s">
-        <v>206</v>
-      </c>
-      <c r="C72" s="23" t="s">
-        <v>70</v>
-      </c>
+      <c r="A72" s="26"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="27"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="26"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="27"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="26"/>
@@ -3455,41 +3395,11 @@
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="26"/>
       <c r="B77" s="38"/>
-      <c r="C77" s="27"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="27"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="26"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="27"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="27"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="27"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
-      <c r="B82" s="38"/>
-      <c r="C82" s="27"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="26"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="28"/>
+      <c r="C77" s="28"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C22" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:C18">
+  <autoFilter ref="A1:C16" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:C12">
     <sortCondition ref="C3"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3502,7 +3412,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3530,16 +3440,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C2" s="5">
-        <v>201902282</v>
+        <v>201903081</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to many things
</commit_message>
<xml_diff>
--- a/ILRG_Hluvukani_A_encontros/ILRG_Hluvukani_A_encontros-media/ILRG_Hluvukani_A_encontros.xlsx
+++ b/ILRG_Hluvukani_A_encontros/ILRG_Hluvukani_A_encontros-media/ILRG_Hluvukani_A_encontros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\Grants\Hluvukani\ODK Forms\ILRG_hluvukani_odk_forms\ILRG_Hluvukani_A_encontros\ILRG_Hluvukani_A_encontros-media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\hluvukani\ODK Forms\ILRG_hluvukani_odk_forms\ILRG_Hluvukani_A_encontros\ILRG_Hluvukani_A_encontros-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A267EA18-D249-43C6-861C-D6ADF17542B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B082ED-4C78-4CB0-B615-E2F3387CEAF0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -784,9 +784,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1031,359 +1038,366 @@
   </borders>
   <cellStyleXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="234" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="234" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1963,7 +1977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2589,11 +2603,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24:XFD26"/>
+      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2986,7 +3000,7 @@
       <c r="B34" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="62" t="s">
         <v>117</v>
       </c>
       <c r="F34" s="48"/>
@@ -2998,7 +3012,7 @@
       <c r="B35" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="62" t="s">
         <v>118</v>
       </c>
       <c r="E35" s="47"/>
@@ -3043,10 +3057,10 @@
       <c r="A39" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="62" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3054,10 +3068,10 @@
       <c r="A40" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="63" t="s">
         <v>217</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="62" t="s">
         <v>122</v>
       </c>
       <c r="E40" s="49"/>
@@ -3067,10 +3081,10 @@
       <c r="A41" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="62" t="s">
         <v>123</v>
       </c>
       <c r="E41" s="49"/>
@@ -3101,7 +3115,7 @@
       <c r="B44" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="61" t="s">
         <v>125</v>
       </c>
       <c r="E44" s="49"/>
@@ -3140,7 +3154,7 @@
       <c r="B47" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="61" t="s">
         <v>126</v>
       </c>
       <c r="E47" s="49"/>
@@ -3153,7 +3167,7 @@
       <c r="B48" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="61" t="s">
         <v>127</v>
       </c>
       <c r="F48" s="48"/>

</xml_diff>